<commit_message>
Renaming and re-doing interval adjustment
</commit_message>
<xml_diff>
--- a/data-raw/eddystore_proc_table.xlsx
+++ b/data-raw/eddystore_proc_table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\0Peter\curr\ECsystem\eddystore\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\plevy\Documents\eddystore\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
   <si>
     <t>siteID</t>
   </si>
@@ -50,12 +50,6 @@
     <t>data_path</t>
   </si>
   <si>
-    <t>proc_filepath</t>
-  </si>
-  <si>
-    <t>/group_workspaces/jasmin2/eddystore/stations/EasterBush/proc/processing.eddypro</t>
-  </si>
-  <si>
     <t>stationID</t>
   </si>
   <si>
@@ -99,6 +93,33 @@
   </si>
   <si>
     <t>/group_workspaces/jasmin2/eddystore/stations/Auchencorth/proc/processing_2007.eddypro</t>
+  </si>
+  <si>
+    <t>/group_workspaces/jasmin2/eddystore/stations/EasterBush/proc/processing1995.eddypro</t>
+  </si>
+  <si>
+    <t>/group_workspaces/jasmin2/eddystore/stations/EasterBush/proc/processing2007.eddypro</t>
+  </si>
+  <si>
+    <t>/group_workspaces/jasmin2/eddystore/stations/EasterBush/proc/processing2013.eddypro</t>
+  </si>
+  <si>
+    <t>project_filepath</t>
+  </si>
+  <si>
+    <t>EB_jasmin</t>
+  </si>
+  <si>
+    <t>EasterBush_jasmin</t>
+  </si>
+  <si>
+    <t>N:/0Peter/curr/ECsystem/eddypro/EB_1995.eddypro</t>
+  </si>
+  <si>
+    <t>N:/0Peter/curr/ECsystem/eddypro/EB_2007.eddypro</t>
+  </si>
+  <si>
+    <t>N:/0Peter/curr/ECsystem/eddypro/EB_2013.eddypro</t>
   </si>
 </sst>
 </file>
@@ -106,7 +127,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -142,7 +163,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G11"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,10 +466,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -457,7 +478,7 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="G1" t="s">
         <v>7</v>
@@ -471,10 +492,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2">
         <v>34700</v>
@@ -482,8 +503,8 @@
       <c r="E2" s="2">
         <v>39082.999305555553</v>
       </c>
-      <c r="F2" t="s">
-        <v>9</v>
+      <c r="F2" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="G2" t="str">
         <f>"/group_workspaces/jasmin2/eddystore/stations/" &amp; $B2 &amp; "/raw_files"</f>
@@ -499,10 +520,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2">
         <v>39083</v>
@@ -510,8 +531,8 @@
       <c r="E3" s="2">
         <v>41274.999305555553</v>
       </c>
-      <c r="F3" t="s">
-        <v>9</v>
+      <c r="F3" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G11" si="0">"/group_workspaces/jasmin2/eddystore/stations/" &amp; $B3 &amp; "/raw_files"</f>
@@ -527,10 +548,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2">
         <v>41275</v>
@@ -538,8 +559,8 @@
       <c r="E4" s="2">
         <v>43831.5</v>
       </c>
-      <c r="F4" t="s">
-        <v>9</v>
+      <c r="F4" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
@@ -555,10 +576,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2">
         <v>42370</v>
@@ -567,7 +588,7 @@
         <v>43831.5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
@@ -583,10 +604,10 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2">
         <v>34700</v>
@@ -595,7 +616,7 @@
         <v>39082.999305555553</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
@@ -611,10 +632,10 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2">
         <v>39083</v>
@@ -623,7 +644,7 @@
         <v>41274.999305555553</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
@@ -639,10 +660,10 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8" s="2">
         <v>41275</v>
@@ -651,7 +672,7 @@
         <v>43831.5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
@@ -667,10 +688,10 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D9" s="2">
         <v>34700</v>
@@ -679,7 +700,7 @@
         <v>39082.999305555553</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
@@ -695,10 +716,10 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D10" s="2">
         <v>39083</v>
@@ -707,7 +728,7 @@
         <v>41274.999305555553</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
@@ -723,10 +744,10 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D11" s="2">
         <v>41275</v>
@@ -735,7 +756,7 @@
         <v>43831.5</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
@@ -745,6 +766,121 @@
         <f t="shared" si="1"/>
         <v>/group_workspaces/jasmin2/eddystore/stations/Whim/output</v>
       </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="2">
+        <v>34700</v>
+      </c>
+      <c r="E12" s="2">
+        <v>39082.999305555553</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" t="str">
+        <f>"/group_workspaces/jasmin2/eddystore/stations/" &amp; $B12 &amp; "/raw_files"</f>
+        <v>/group_workspaces/jasmin2/eddystore/stations/EasterBush_jasmin/raw_files</v>
+      </c>
+      <c r="H12" t="str">
+        <f>"/group_workspaces/jasmin2/eddystore/stations/" &amp; $B12 &amp; "/output"</f>
+        <v>/group_workspaces/jasmin2/eddystore/stations/EasterBush_jasmin/output</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="2">
+        <v>39083</v>
+      </c>
+      <c r="E13" s="2">
+        <v>41274.999305555553</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" ref="G13:G15" si="2">"/group_workspaces/jasmin2/eddystore/stations/" &amp; $B13 &amp; "/raw_files"</f>
+        <v>/group_workspaces/jasmin2/eddystore/stations/EasterBush_jasmin/raw_files</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" ref="H13:H15" si="3">"/group_workspaces/jasmin2/eddystore/stations/" &amp; $B13 &amp; "/output"</f>
+        <v>/group_workspaces/jasmin2/eddystore/stations/EasterBush_jasmin/output</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="2">
+        <v>41275</v>
+      </c>
+      <c r="E14" s="2">
+        <v>43831.5</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="2"/>
+        <v>/group_workspaces/jasmin2/eddystore/stations/EasterBush_jasmin/raw_files</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="3"/>
+        <v>/group_workspaces/jasmin2/eddystore/stations/EasterBush_jasmin/output</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="2">
+        <v>42370</v>
+      </c>
+      <c r="E15" s="2">
+        <v>43831.5</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="2"/>
+        <v>/group_workspaces/jasmin2/eddystore/stations/EasterBush_jasmin/raw_files</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="3"/>
+        <v>/group_workspaces/jasmin2/eddystore/stations/EasterBush_jasmin/output</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>